<commit_message>
Adding figure code, adding bibliography 3/26
</commit_message>
<xml_diff>
--- a/Data_Bibliography.xlsx
+++ b/Data_Bibliography.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26322"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate.sharepoint.com/sites/Section_SS23-CMSE-495-001-223211859-EL-32-A26-QSIDE-Human_Trafficking/Shared Documents/QSIDE-Human_Trafficking/Team Member Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{934B1104-DCD3-4302-97D5-54E8DBD93D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED17CCA8-B27D-488F-8987-8439BEADAC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="3360" yWindow="340" windowWidth="15780" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="142">
   <si>
     <t>Title</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>This resource contains information on various governmental committees around Michigan dealing with Human Trafficking. Contact names and department names for these prevention/prosecution resources can be found. Also includes arrest data for a small window in time relating to human trafficking.</t>
+  </si>
+  <si>
+    <t>Law enforcement</t>
   </si>
   <si>
     <t>J</t>
@@ -121,6 +124,9 @@
     <t>This resource contains information on various governmental committees around Michigan dealing with Human Trafficking. Contact names and department names for these prevention/prosecution resources can be found. Some updates from the previous year's report</t>
   </si>
   <si>
+    <t>travel</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bureau of Justice Statistics – Human Trafficking Data Collection Activities, 2021 </t>
   </si>
   <si>
@@ -232,13 +238,22 @@
     <t>Why are You Here? Modeling Illicit Massage Business Location Characteristics with Machine Learning</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.tandfonline.com/doi/full/10.1080/23322705.2021.1982238  </t>
+    <t>https://www2.census.gov/geo/maps/metroarea/us_wall/Feb2013/cbsa_us_0213.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This paper lead to another source (https://www.tandfonline.com/doi/full/10.1080/23322705.2017.1374080?scroll=top&amp;needAccess=true&amp;role=tab) focused in texas in which they used a website called RubMaps where users would talk abotu their experience at illicit massage businesses; upon trying to access this i was not able to; s o maybe qside has a proxy or vpn? Census demographic data were assigned to each IMB in the data set by establishing the “neighborhood” for each location. The IMB neighborhood was defined as all of the census tracts that fell within 0.5 miles of each IMB. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.tandfonline.com/doi/full/10.1080/23322705.2021.1982238 https://www.census.gov/programs-surveys/acs/technical-documentation/table-and-geography-changes/2013/1-year.html#par_textimage_1 </t>
   </si>
   <si>
     <t>Michigan, Texas</t>
   </si>
   <si>
     <t xml:space="preserve">Based on addresses web-scraped weekly from online advertisements over 6 months, we modeled illicit massage business prevalence at the census tract and county levels </t>
+  </si>
+  <si>
+    <t>Connected with the census and illicit massage businesses; there are factors connected with race, neighborhood</t>
   </si>
   <si>
     <t>National Child Abuse and Neglect Data System</t>
@@ -347,13 +362,16 @@
     <t>SAIPE School District Estimates for 2021</t>
   </si>
   <si>
+    <t>Text filescontaining poverty levels in school districts nationwide are avalible to download in article</t>
+  </si>
+  <si>
     <t>SAIPE School District Estimates for 2021 (census.gov)</t>
   </si>
   <si>
     <t>Michigan, Welfare</t>
   </si>
   <si>
-    <t>Multiple tables containing details on estimates of population and poverty in different school stricts across the country</t>
+    <t>Multiple tables containing details on estimates of population and poverty in different school stricts across the country. The 2021 estimates are consistent with the population controls and income concepts used in the 2021 American Community Survey single-year estimates.</t>
   </si>
   <si>
     <t>The table contains data that can be useful in understanding which school districts, and potentially which states have higher risks of poverty</t>
@@ -368,6 +386,9 @@
     <t>Excel Data Tables</t>
   </si>
   <si>
+    <t>State IRS, State/Country SNAP benefits, State/county poverty data found on Article link</t>
+  </si>
+  <si>
     <t>https://www.census.gov/data/datasets/time-series/demo/saipe/model-tables.html</t>
   </si>
   <si>
@@ -386,13 +407,16 @@
     <t>PDF, data from study</t>
   </si>
   <si>
+    <t>There were 235 offenses relating to sex trafficking (198 trafficking of persons and 37 compelling prostitution offenses) recorded by the APD during 2013–2015. (APD = Austin Police Department --&gt; data from there?), but data for roads and SOB locations now unavailable</t>
+  </si>
+  <si>
     <t>https://www.sciencedirect.com/science/article/pii/S0047235218301934?casa_token=rYOwb2PB5iQAAAAA:Y-T55DLYZnsrm1n3ISGdgRsT2puq6rx9yok6aJrrlifMXTTRnUTZswXZ1cthVxiu9C2woiAewEY</t>
   </si>
   <si>
     <t>urban neighborhood, Texas, geography, interstate highway</t>
   </si>
   <si>
-    <t>extent of spatial concentration of sex trafficking; there was a significant cluster of sex trafficking offenses associated with the proximity to the interstate highway</t>
+    <t>Extent of spatial concentration of sex trafficking; there was a significant cluster of sex trafficking offenses associated with the proximity to the interstate highway</t>
   </si>
   <si>
     <t>data science analysis in Texas that shows a connections with geographic clustering factors that are related to HT and that don't increase the risk</t>
@@ -410,22 +434,20 @@
     <t>health care provider,     Child sexual abuse, labor trafficking, legislative review, mandatory education, mandatory reporting, sex trafficking</t>
   </si>
   <si>
-    <t>systematic review of U.S. laws that address education about human trafficking and/or mandatory reporting requirements that affect healthcare providers and other professionals across the United States</t>
+    <t>Systematic review of U.S. laws that address education about human trafficking and/or mandatory reporting requirements that affect healthcare providers and other professionals across the United States</t>
   </si>
   <si>
     <t>goes through 13 states laws + the results can help future physicians and mandated reporters identify HT better</t>
   </si>
   <si>
-    <t>Michigan's First Human Trafficking Court</t>
-  </si>
-  <si>
-    <t>https://heinonline-org.proxy1.cl.msu.edu/HOL/Page?collection=journals&amp;handle=hein.journals/stlulj60&amp;id=110&amp;men_tab=srchresults</t>
-  </si>
-  <si>
     <t>Victim or Whore: The Similarities and Differences between Victim's Experiences of Domestic Violence and Sex Trafficking</t>
   </si>
   <si>
     <t>https://www.tandfonline.com/doi/full/10.1080/10911359.2013.840552?casa_token=eJYIpCD76LwAAAAA%3ApYCgbzESyoXiblqOmLB_OK42O8T69cl6XlHuDIwcATAEisQYZTjYwcX0B0ymEEDic3wMToTcO7k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    Sex trafficking, domestic violence, victim, violence against women</t>
   </si>
   <si>
     <t>Difference between domestic violence and HT</t>
@@ -978,11 +1000,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="D18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
@@ -990,12 +1012,12 @@
     <col min="1" max="1" width="18" style="8" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" style="5" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" style="14" customWidth="1"/>
     <col min="5" max="5" width="34.85546875" style="17" customWidth="1"/>
     <col min="6" max="6" width="24.140625" style="5" customWidth="1"/>
     <col min="7" max="7" width="39.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="36.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="3"/>
+    <col min="9" max="9" width="18.85546875" style="3" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" style="5" customWidth="1"/>
     <col min="11" max="11" width="22.7109375" style="3" customWidth="1"/>
     <col min="12" max="13" width="9.140625" style="3"/>
@@ -1060,449 +1082,479 @@
       <c r="H2" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="I2" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="J2" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="121.5">
       <c r="A3" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="J3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="121.5">
+      <c r="A4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="152.25">
-      <c r="A4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="J4" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="152.25">
       <c r="A5" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="106.5">
       <c r="A6" s="8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="76.5">
       <c r="A7" s="8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="106.5">
       <c r="A8" s="8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="106.5">
       <c r="A9" s="8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E9" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="366">
+      <c r="A10" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="91.5">
-      <c r="A10" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>54</v>
+      <c r="C10" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>63</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="152.25">
       <c r="A11" s="8" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="106.5">
       <c r="A12" s="8" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="106.5">
       <c r="A13" s="8" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="121.5">
       <c r="A14" s="8" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="106.5">
       <c r="A15" s="8" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="60.75">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="106.5">
       <c r="A16" s="8" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>102</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="91.5">
       <c r="A17" s="8" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>103</v>
+        <v>109</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>110</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="106.5">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="229.5">
       <c r="A18" s="8" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>109</v>
+        <v>116</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>117</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="152.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="137.25">
       <c r="A19" s="8" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="76.5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="106.5">
       <c r="A20" s="8" t="s">
-        <v>120</v>
+        <v>128</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>121</v>
+        <v>129</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>131</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="106.5">
-      <c r="A21" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>125</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="E21" s="16"/>
     </row>
     <row r="22" spans="1:11"/>
-    <row r="23" spans="1:11"/>
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{C16078C6-0E4B-4C47-8598-644D7A59B756}"/>
@@ -1516,7 +1568,7 @@
     <hyperlink ref="E7" r:id="rId6" location=":~:text=Web%20Chat%3A%2095-,Cases,were%20identified%20in%20these%20cases" xr:uid="{20F3D778-9EB7-4100-B544-0F629C59862C}"/>
     <hyperlink ref="E8" r:id="rId7" xr:uid="{2E35C3D3-8758-471E-A920-B0F8C0D6150D}"/>
     <hyperlink ref="E9" r:id="rId8" xr:uid="{551E7F0E-49CF-4B20-9AA1-E3823A3A283A}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{9E268F8F-10BC-4911-8130-DA2CE02F36AF}"/>
+    <hyperlink ref="E10" r:id="rId9" location="par_textimage_1" xr:uid="{9E268F8F-10BC-4911-8130-DA2CE02F36AF}"/>
     <hyperlink ref="E11" r:id="rId10" xr:uid="{1C162764-94DC-4ACB-804C-95B4608D6418}"/>
     <hyperlink ref="E12" r:id="rId11" xr:uid="{697C878B-56A9-49CF-812E-17809EC1BCEF}"/>
     <hyperlink ref="E13" r:id="rId12" xr:uid="{74C4920A-43D1-433E-B7E9-48DA797A2663}"/>
@@ -1524,16 +1576,16 @@
     <hyperlink ref="E15" r:id="rId14" xr:uid="{8C9ED3CD-1849-49F2-A0A8-8B19390AC75A}"/>
     <hyperlink ref="E16" r:id="rId15" xr:uid="{7098B384-708E-4710-8871-E064BB37BBEC}"/>
     <hyperlink ref="E17" r:id="rId16" xr:uid="{333AF3A0-26F9-4419-BBC2-BF8B2856140B}"/>
-    <hyperlink ref="E20" r:id="rId17" xr:uid="{EA14D901-E73E-BA43-98A2-F9866BC9B446}"/>
-    <hyperlink ref="E21" r:id="rId18" xr:uid="{6FE8F2F1-2963-CF4B-937C-D8001722EBBE}"/>
-    <hyperlink ref="C9" r:id="rId19" xr:uid="{C0C44B39-ED24-4CB7-8567-36BDE64C048B}"/>
-    <hyperlink ref="C5" r:id="rId20" xr:uid="{EBB03B43-6801-41CF-B28C-67B4021EBFA4}"/>
-    <hyperlink ref="C4" r:id="rId21" xr:uid="{48E51C56-2EE1-4586-B1D8-8D9997236B46}"/>
-    <hyperlink ref="C12" r:id="rId22" xr:uid="{8026EAB3-3588-4AD6-8172-4E36C92FA1CE}"/>
-    <hyperlink ref="C14" r:id="rId23" xr:uid="{936134BF-6EED-4C2B-901C-A0DF4F02AC02}"/>
-    <hyperlink ref="C15" r:id="rId24" location="list-tab-1036221584" xr:uid="{7C8040CD-0183-4147-A3AD-BB43AD6220C8}"/>
-    <hyperlink ref="E18" r:id="rId25" xr:uid="{8367973A-61D7-4F56-802C-B742E5D509D9}"/>
-    <hyperlink ref="E19" r:id="rId26" xr:uid="{A1A44711-DE29-45C1-AB73-FCB76B0C358D}"/>
+    <hyperlink ref="E20" r:id="rId17" xr:uid="{6FE8F2F1-2963-CF4B-937C-D8001722EBBE}"/>
+    <hyperlink ref="C9" r:id="rId18" xr:uid="{C0C44B39-ED24-4CB7-8567-36BDE64C048B}"/>
+    <hyperlink ref="C5" r:id="rId19" xr:uid="{EBB03B43-6801-41CF-B28C-67B4021EBFA4}"/>
+    <hyperlink ref="C4" r:id="rId20" xr:uid="{48E51C56-2EE1-4586-B1D8-8D9997236B46}"/>
+    <hyperlink ref="C12" r:id="rId21" xr:uid="{8026EAB3-3588-4AD6-8172-4E36C92FA1CE}"/>
+    <hyperlink ref="C14" r:id="rId22" xr:uid="{936134BF-6EED-4C2B-901C-A0DF4F02AC02}"/>
+    <hyperlink ref="C15" r:id="rId23" location="list-tab-1036221584" xr:uid="{7C8040CD-0183-4147-A3AD-BB43AD6220C8}"/>
+    <hyperlink ref="E18" r:id="rId24" xr:uid="{8367973A-61D7-4F56-802C-B742E5D509D9}"/>
+    <hyperlink ref="E19" r:id="rId25" xr:uid="{A1A44711-DE29-45C1-AB73-FCB76B0C358D}"/>
+    <hyperlink ref="C10" r:id="rId26" xr:uid="{0F3DACF6-400C-4650-AD28-B70FA65152EB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1554,47 +1606,47 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="11" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1603,12 +1655,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1789,13 +1838,16 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34C456AF-73FA-4F35-AC7E-80993F768A17}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD7481EB-B433-4263-8C3D-876818642452}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1803,5 +1855,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD7481EB-B433-4263-8C3D-876818642452}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34C456AF-73FA-4F35-AC7E-80993F768A17}"/>
 </file>
</xml_diff>